<commit_message>
refacut review report, adaugat modificari
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R1kK\Desktop\teme\sem 6\URSS\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581A3701-5311-42CD-B169-5153526D85A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99415399-C2AD-4E38-9CF7-9FF2E8A72F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{182114F5-4D7A-472B-AE68-3AF703D642CB}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{182114F5-4D7A-472B-AE68-3AF703D642CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>i.</t>
   </si>
@@ -70,64 +70,64 @@
     <t>Observatii</t>
   </si>
   <si>
-    <t>Lab01_Requirements</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
-    <t>no requirements</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
-    <t>Lab01_Architectural</t>
-  </si>
-  <si>
     <t>A3</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>no classes (functional React)</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
     <t>A10</t>
   </si>
   <si>
-    <t>Lab01_Program</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>no loops</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>no variable dimensions required</t>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>no input validation</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>plaintext used, not localization</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>no requirements at all</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>not all requirements completed</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>not all requirements implemented</t>
+  </si>
+  <si>
+    <t>requirements should be better described</t>
+  </si>
+  <si>
+    <t>more detail on user experience</t>
+  </si>
+  <si>
+    <t>custom documents not covered by requirements</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,25 +211,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -244,9 +231,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3284B622-C8B0-45E2-BA57-AE3BD5F66148}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,6 +592,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -620,89 +607,96 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>20</v>
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -710,83 +704,31 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C17" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>